<commit_message>
store curated data in appropriate directory #25
</commit_message>
<xml_diff>
--- a/documents/test.xlsx
+++ b/documents/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonnemanm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn_000\Documents\GitHub\data_portal\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DF8736-438C-4C86-A4D7-01A333BFC26C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="3"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11505" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="146">
   <si>
     <t>sheet</t>
   </si>
@@ -516,9 +517,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>AFDS</t>
   </si>
   <si>
@@ -600,7 +598,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -1215,6 +1213,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1250,6 +1265,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1425,7 +1457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -1551,19 +1583,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="195" yWindow="491" count="10">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of person to be contacted" sqref="A3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data entry person(s)" sqref="A5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the version of the MarineGEO protocol referenced to collect these data" sqref="A9"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data of final data entry" sqref="A6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of any other person(s) involved" sqref="A7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please note any special cirucumstances, unusual findings, data abnormalities, etc…that might impact the interpretation of these data" sqref="A8"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the protocol" sqref="A2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="E-mail of the contact person" sqref="A4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The version number of this workbook" sqref="A10"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seriously, feel free to contact us!" sqref="A11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of person to be contacted" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data entry person(s)" sqref="A5" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the version of the MarineGEO protocol referenced to collect these data" sqref="A9" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data of final data entry" sqref="A6" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of any other person(s) involved" sqref="A7" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please note any special cirucumstances, unusual findings, data abnormalities, etc…that might impact the interpretation of these data" sqref="A8" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the protocol" sqref="A2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="E-mail of the contact person" sqref="A4" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The version number of this workbook" sqref="A10" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seriously, feel free to contact us!" sqref="A11" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1571,7 +1603,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -1888,21 +1920,21 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="E1 G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="F1 H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Site depth in meters. _x000a__x000a_For sites spanning a depth range, please provide a single, average depth." sqref="I1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any comments reguarding the sampling location" sqref="J1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="E1 G1" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="F1 H1" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Site depth in meters. _x000a__x000a_For sites spanning a depth range, please provide a single, average depth." sqref="I1" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any comments reguarding the sampling location" sqref="J1" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -2355,28 +2387,28 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cover codes are 1, 2, 3, 4, 5 where:_x000d__x000a_1 = 0-5%_x000d__x000a_2 = 5-25%_x000d__x000a_3 = 25-50%_x000d__x000a_4 = 50-75%_x000d__x000a_5 = 75-100%" sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="F1" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cover codes are 1, 2, 3, 4, 5 where:_x000d__x000a_1 = 0-5%_x000d__x000a_2 = 5-25%_x000d__x000a_3 = 25-50%_x000d__x000a_4 = 50-75%_x000d__x000a_5 = 75-100%" sqref="G1" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1" xr:uid="{00000000-0002-0000-0200-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0200-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0200-000006000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2573,11 +2605,11 @@
       <c r="H6" t="s">
         <v>119</v>
       </c>
-      <c r="I6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>120</v>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2911,22 +2943,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <dataValidations count="9">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1:G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Were there obivious grazing scars present in the quadrat, Y or N?" sqref="H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass shoots within the quadrat." sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass flowers (if any) present  within the qudrat._x000d__x000a__x000d__x000a_Remember - Zeros are data! Please enter 0 if no seagrass flowers were present." sqref="I1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass fruits (if any) present  within the qudrat._x000a__x000a_Remember - Zeros are data! Please enter 0 if no seagrass flowers were present." sqref="J1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1:G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Were there obivious grazing scars present in the quadrat, Y or N?" sqref="H1" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass shoots within the quadrat." sqref="G1" xr:uid="{00000000-0002-0000-0300-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass flowers (if any) present  within the qudrat._x000d__x000a__x000d__x000a_Remember - Zeros are data! Please enter 0 if no seagrass flowers were present." sqref="I1" xr:uid="{00000000-0002-0000-0300-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass fruits (if any) present  within the qudrat._x000a__x000a_Remember - Zeros are data! Please enter 0 if no seagrass flowers were present." sqref="J1" xr:uid="{00000000-0002-0000-0300-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0300-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1" xr:uid="{00000000-0002-0000-0300-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0300-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0300-000008000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -2986,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -3009,7 +3041,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -3032,7 +3064,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -3055,7 +3087,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G5">
         <v>12</v>
@@ -3078,7 +3110,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -3101,7 +3133,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -3124,7 +3156,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G8">
         <v>0.5</v>
@@ -3147,7 +3179,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G9">
         <v>18</v>
@@ -3170,7 +3202,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G10">
         <v>0.24660000000000001</v>
@@ -3379,20 +3411,20 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The size of any mobile inverts to the nearest millimeter. If more than one individual of a given taxon is present in a single quadrat, enter a single row for each individual." sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="F1" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The size of any mobile inverts to the nearest millimeter. If more than one individual of a given taxon is present in a single quadrat, enter a single row for each individual." sqref="G1" xr:uid="{00000000-0002-0000-0400-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0400-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1" xr:uid="{00000000-0002-0000-0400-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0400-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0400-000006000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -3419,74 +3451,74 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3494,7 +3526,7 @@
         <v>110</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3502,7 +3534,7 @@
         <v>111</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3510,7 +3542,7 @@
         <v>112</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3518,7 +3550,7 @@
         <v>113</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3526,7 +3558,7 @@
         <v>114</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -3534,7 +3566,7 @@
         <v>115</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3542,7 +3574,7 @@
         <v>116</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3550,20 +3582,20 @@
         <v>117</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique identifier used to identify a single taxon. This column should include ALL uniquie TaxonID entries from the 'data' sheet" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Indicate taxa's scientific name using standard scientific nomenclature." sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique identifier used to identify a single taxon. This column should include ALL uniquie TaxonID entries from the 'data' sheet" sqref="A1" xr:uid="{00000000-0002-0000-0500-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Indicate taxa's scientific name using standard scientific nomenclature." sqref="B1" xr:uid="{00000000-0002-0000-0500-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -4584,14 +4616,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The sheet in which the field occurs" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the field being defined" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field definition" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B18:B21"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="B31 B47"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The sheet in which the field occurs" sqref="A1" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the field being defined" sqref="B1" xr:uid="{00000000-0002-0000-0600-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field definition" sqref="C1" xr:uid="{00000000-0002-0000-0600-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1" xr:uid="{00000000-0002-0000-0600-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1" xr:uid="{00000000-0002-0000-0600-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1" xr:uid="{00000000-0002-0000-0600-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B18:B21" xr:uid="{00000000-0002-0000-0600-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="B31 B47" xr:uid="{00000000-0002-0000-0600-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
multiple file submissions saved according to individual QA results
</commit_message>
<xml_diff>
--- a/documents/test.xlsx
+++ b/documents/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11505" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="147">
   <si>
     <t>sheet</t>
   </si>
@@ -1432,7 +1432,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -1483,7 +1483,7 @@
         <v>65</v>
       </c>
       <c r="B6" s="12">
-        <v>43480</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -2372,9 +2372,9 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2574,8 +2574,8 @@
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6" s="1">
-        <v>0</v>
+      <c r="J6" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2930,9 +2930,9 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>